<commit_message>
Update Geospatial module & station record mapping
</commit_message>
<xml_diff>
--- a/WebScraping/data/Station_Records.xlsx
+++ b/WebScraping/data/Station_Records.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fm/ISSS608-G6/WebScraping/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\thuphuong1110\Group_project\ISSS608-G6\ISSS608-G6\WebScraping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83794653-56DD-A94E-BC80-6F01F5930FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B65D0F5-309A-445B-A231-CE11DF24B92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="800" windowWidth="38320" windowHeight="23120" xr2:uid="{CB4FE421-B271-4A9C-BCDD-13479AD81A22}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CB4FE421-B271-4A9C-BCDD-13479AD81A22}"/>
   </bookViews>
   <sheets>
     <sheet name="Station" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Station!$A$1:$E$64</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -56,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="134">
   <si>
     <t>Admiralty</t>
   </si>
@@ -361,9 +364,6 @@
     <t>S94</t>
   </si>
   <si>
-    <t>Pasir Ris (Central)</t>
-  </si>
-  <si>
     <t>S29</t>
   </si>
   <si>
@@ -440,25 +440,39 @@
   </si>
   <si>
     <t>S110</t>
+  </si>
+  <si>
+    <t>Lat</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Pasir Ris Central</t>
+  </si>
+  <si>
+    <t>Station Type</t>
+  </si>
+  <si>
+    <t>Full AWS Station</t>
+  </si>
+  <si>
+    <t>Closed Station</t>
+  </si>
+  <si>
+    <t>Rainfall Station</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -484,7 +498,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,530 +833,991 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D26EEE-2AC8-46D9-9440-40AE878315C7}">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>1.4439</v>
+      </c>
+      <c r="D2">
+        <v>103.7854</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>1.3793</v>
+      </c>
+      <c r="D4">
+        <v>103.85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>1.3087</v>
+      </c>
+      <c r="D7">
+        <v>103.818</v>
+      </c>
+      <c r="E7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>1.3823000000000001</v>
+      </c>
+      <c r="D9">
+        <v>103.7607</v>
+      </c>
+      <c r="E9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1.3190999999999999</v>
+      </c>
+      <c r="D10">
+        <v>103.8193</v>
+      </c>
+      <c r="E10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>1.2841</v>
+      </c>
+      <c r="D11">
+        <v>103.78879999999999</v>
+      </c>
+      <c r="E11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>1.3677999999999999</v>
+      </c>
+      <c r="D13">
+        <v>103.9823</v>
+      </c>
+      <c r="E13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>1.3821000000000001</v>
+      </c>
+      <c r="D14">
+        <v>103.7381</v>
+      </c>
+      <c r="E14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>1.3729</v>
+      </c>
+      <c r="D15">
+        <v>103.72239999999999</v>
+      </c>
+      <c r="E15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>50</v>
       </c>
       <c r="B16" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>1.3318000000000001</v>
+      </c>
+      <c r="D17">
+        <v>103.7762</v>
+      </c>
+      <c r="E17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>51</v>
       </c>
       <c r="B18" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>1.3132999999999999</v>
+      </c>
+      <c r="D19">
+        <v>103.962</v>
+      </c>
+      <c r="E19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>53</v>
       </c>
       <c r="B21" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>1.3458000000000001</v>
+      </c>
+      <c r="D22">
+        <v>103.68170000000001</v>
+      </c>
+      <c r="E22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>1.2542</v>
+      </c>
+      <c r="D23">
+        <v>103.6741</v>
+      </c>
+      <c r="E23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>1.3082</v>
+      </c>
+      <c r="D24">
+        <v>103.71</v>
+      </c>
+      <c r="E24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>54</v>
       </c>
       <c r="B25" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>1.2923</v>
+      </c>
+      <c r="D26">
+        <v>103.78149999999999</v>
+      </c>
+      <c r="E26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>61</v>
       </c>
       <c r="B27" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>1.4387000000000001</v>
+      </c>
+      <c r="D28">
+        <v>103.736</v>
+      </c>
+      <c r="E28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>1.4388000000000001</v>
+      </c>
+      <c r="D29">
+        <v>103.7017</v>
+      </c>
+      <c r="E29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>1.37</v>
+      </c>
+      <c r="D30">
+        <v>103.8271</v>
+      </c>
+      <c r="E30" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>1.3418000000000001</v>
+      </c>
+      <c r="D31">
+        <v>103.8339</v>
+      </c>
+      <c r="E31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>1.4067000000000001</v>
+      </c>
+      <c r="D32">
+        <v>103.78319999999999</v>
+      </c>
+      <c r="E32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>8</v>
       </c>
       <c r="B33" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>1.2799</v>
+      </c>
+      <c r="D33">
+        <v>103.8703</v>
+      </c>
+      <c r="E33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>1.3049999999999999</v>
+      </c>
+      <c r="D34">
+        <v>103.91119999999999</v>
+      </c>
+      <c r="E34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>9</v>
       </c>
       <c r="B35" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>1.3106</v>
+      </c>
+      <c r="D35">
+        <v>103.8365</v>
+      </c>
+      <c r="E35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>33</v>
       </c>
       <c r="B36" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="D36">
+        <v>103.8622</v>
+      </c>
+      <c r="E36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>10</v>
       </c>
       <c r="B37" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>1.2824</v>
+      </c>
+      <c r="D37">
+        <v>103.75449999999999</v>
+      </c>
+      <c r="E37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="C38">
+        <v>1.3865000000000001</v>
+      </c>
+      <c r="D38">
+        <v>103.9413</v>
+      </c>
+      <c r="E38" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>1.3678999999999999</v>
+      </c>
+      <c r="D39">
+        <v>103.94889999999999</v>
+      </c>
+      <c r="E39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="C40">
+        <v>1.3571</v>
+      </c>
+      <c r="D40">
+        <v>103.9037</v>
+      </c>
+      <c r="E40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="C41">
+        <v>1.4168000000000001</v>
+      </c>
+      <c r="D41">
+        <v>103.96729999999999</v>
+      </c>
+      <c r="E41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="C42">
+        <v>1.4028</v>
+      </c>
+      <c r="D42">
+        <v>103.90949999999999</v>
+      </c>
+      <c r="E42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="C43">
+        <v>1.2937000000000001</v>
+      </c>
+      <c r="D43">
+        <v>103.81270000000001</v>
+      </c>
+      <c r="E43" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="C44">
+        <v>1.4167000000000001</v>
+      </c>
+      <c r="D44">
+        <v>103.86499999999999</v>
+      </c>
+      <c r="E44" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="C45">
+        <v>1.1901999999999999</v>
+      </c>
+      <c r="D45">
+        <v>103.7657</v>
+      </c>
+      <c r="E45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="C46">
+        <v>1.425</v>
+      </c>
+      <c r="D46">
+        <v>103.82</v>
+      </c>
+      <c r="E46" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="C47">
+        <v>1.2503</v>
+      </c>
+      <c r="D47">
+        <v>103.8275</v>
+      </c>
+      <c r="E47" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="C48">
+        <v>1.3376999999999999</v>
+      </c>
+      <c r="D48">
+        <v>103.86620000000001</v>
+      </c>
+      <c r="E48" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="E49" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>38</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="C50">
+        <v>1.3443000000000001</v>
+      </c>
+      <c r="D50">
+        <v>103.94410000000001</v>
+      </c>
+      <c r="E50" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>39</v>
       </c>
       <c r="B51" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="C51">
+        <v>1.3003</v>
+      </c>
+      <c r="D51">
+        <v>103.8372</v>
+      </c>
+      <c r="E51" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="C52">
+        <v>1.3406</v>
+      </c>
+      <c r="D52">
+        <v>103.8882</v>
+      </c>
+      <c r="E52" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>40</v>
       </c>
       <c r="B53" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="C53">
+        <v>1.3069999999999999</v>
+      </c>
+      <c r="D53">
+        <v>103.8907</v>
+      </c>
+      <c r="E53" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>56</v>
       </c>
       <c r="B54" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="E54" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="C55">
+        <v>1.3857999999999999</v>
+      </c>
+      <c r="D55">
+        <v>103.7119</v>
+      </c>
+      <c r="E55" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="C56">
+        <v>1.3416999999999999</v>
+      </c>
+      <c r="D56">
+        <v>103.8515</v>
+      </c>
+      <c r="E56" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="C57">
+        <v>1.3199000000000001</v>
+      </c>
+      <c r="D57">
+        <v>103.6613</v>
+      </c>
+      <c r="E57" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>19</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="C58">
+        <v>1.2938000000000001</v>
+      </c>
+      <c r="D58">
+        <v>103.61839999999999</v>
+      </c>
+      <c r="E58" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="E59" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>43</v>
       </c>
       <c r="B60" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="E60" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>44</v>
       </c>
       <c r="B61" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="E61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="E62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>45</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="E63" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>59</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="E64" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E64" xr:uid="{A9D26EEE-2AC8-46D9-9440-40AE878315C7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B64">
     <sortCondition ref="A1:A64"/>
   </sortState>

</xml_diff>

<commit_message>
Update Station records mapping
</commit_message>
<xml_diff>
--- a/WebScraping/data/Station_Records.xlsx
+++ b/WebScraping/data/Station_Records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\thuphuong1110\Group_project\ISSS608-G6\ISSS608-G6\WebScraping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B65D0F5-309A-445B-A231-CE11DF24B92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F993EF39-ABC4-41B5-998F-3369D290FF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CB4FE421-B271-4A9C-BCDD-13479AD81A22}"/>
   </bookViews>
@@ -451,9 +451,6 @@
     <t>Pasir Ris Central</t>
   </si>
   <si>
-    <t>Station Type</t>
-  </si>
-  <si>
     <t>Full AWS Station</t>
   </si>
   <si>
@@ -461,6 +458,9 @@
   </si>
   <si>
     <t>Rainfall Station</t>
+  </si>
+  <si>
+    <t>Station_Type</t>
   </si>
 </sst>
 </file>
@@ -496,9 +496,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,7 +834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D26EEE-2AC8-46D9-9440-40AE878315C7}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -843,10 +844,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>63</v>
       </c>
       <c r="C1" t="s">
@@ -856,7 +857,7 @@
         <v>128</v>
       </c>
       <c r="E1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -873,7 +874,7 @@
         <v>103.7854</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -884,7 +885,7 @@
         <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -901,7 +902,7 @@
         <v>103.85</v>
       </c>
       <c r="E4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -912,7 +913,7 @@
         <v>71</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -923,7 +924,7 @@
         <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -940,7 +941,7 @@
         <v>103.818</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -951,7 +952,7 @@
         <v>69</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -968,7 +969,7 @@
         <v>103.7607</v>
       </c>
       <c r="E9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -985,7 +986,7 @@
         <v>103.8193</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1002,7 +1003,7 @@
         <v>103.78879999999999</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -1013,7 +1014,7 @@
         <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1030,7 +1031,7 @@
         <v>103.9823</v>
       </c>
       <c r="E13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1047,7 +1048,7 @@
         <v>103.7381</v>
       </c>
       <c r="E14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1064,7 +1065,7 @@
         <v>103.72239999999999</v>
       </c>
       <c r="E15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1075,7 +1076,7 @@
         <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1092,7 +1093,7 @@
         <v>103.7762</v>
       </c>
       <c r="E17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1103,7 +1104,7 @@
         <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1120,7 +1121,7 @@
         <v>103.962</v>
       </c>
       <c r="E19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1131,7 +1132,7 @@
         <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1142,7 +1143,7 @@
         <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1159,7 +1160,7 @@
         <v>103.68170000000001</v>
       </c>
       <c r="E22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1176,7 +1177,7 @@
         <v>103.6741</v>
       </c>
       <c r="E23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1193,7 +1194,7 @@
         <v>103.71</v>
       </c>
       <c r="E24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1204,7 +1205,7 @@
         <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1221,7 +1222,7 @@
         <v>103.78149999999999</v>
       </c>
       <c r="E26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1232,7 +1233,7 @@
         <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1249,7 +1250,7 @@
         <v>103.736</v>
       </c>
       <c r="E28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1266,7 +1267,7 @@
         <v>103.7017</v>
       </c>
       <c r="E29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1283,7 +1284,7 @@
         <v>103.8271</v>
       </c>
       <c r="E30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1300,7 +1301,7 @@
         <v>103.8339</v>
       </c>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1317,7 +1318,7 @@
         <v>103.78319999999999</v>
       </c>
       <c r="E32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1334,7 +1335,7 @@
         <v>103.8703</v>
       </c>
       <c r="E33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1351,7 +1352,7 @@
         <v>103.91119999999999</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1368,7 +1369,7 @@
         <v>103.8365</v>
       </c>
       <c r="E35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1385,7 +1386,7 @@
         <v>103.8622</v>
       </c>
       <c r="E36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1402,7 +1403,7 @@
         <v>103.75449999999999</v>
       </c>
       <c r="E37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1419,7 +1420,7 @@
         <v>103.9413</v>
       </c>
       <c r="E38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1436,7 +1437,7 @@
         <v>103.94889999999999</v>
       </c>
       <c r="E39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1453,7 +1454,7 @@
         <v>103.9037</v>
       </c>
       <c r="E40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1470,7 +1471,7 @@
         <v>103.96729999999999</v>
       </c>
       <c r="E41" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1487,7 +1488,7 @@
         <v>103.90949999999999</v>
       </c>
       <c r="E42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1504,7 +1505,7 @@
         <v>103.81270000000001</v>
       </c>
       <c r="E43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -1521,7 +1522,7 @@
         <v>103.86499999999999</v>
       </c>
       <c r="E44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -1538,7 +1539,7 @@
         <v>103.7657</v>
       </c>
       <c r="E45" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -1555,7 +1556,7 @@
         <v>103.82</v>
       </c>
       <c r="E46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -1572,7 +1573,7 @@
         <v>103.8275</v>
       </c>
       <c r="E47" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -1589,7 +1590,7 @@
         <v>103.86620000000001</v>
       </c>
       <c r="E48" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -1600,7 +1601,7 @@
         <v>126</v>
       </c>
       <c r="E49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -1617,7 +1618,7 @@
         <v>103.94410000000001</v>
       </c>
       <c r="E50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -1634,7 +1635,7 @@
         <v>103.8372</v>
       </c>
       <c r="E51" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -1651,7 +1652,7 @@
         <v>103.8882</v>
       </c>
       <c r="E52" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
@@ -1668,7 +1669,7 @@
         <v>103.8907</v>
       </c>
       <c r="E53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -1679,7 +1680,7 @@
         <v>114</v>
       </c>
       <c r="E54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -1696,7 +1697,7 @@
         <v>103.7119</v>
       </c>
       <c r="E55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -1713,7 +1714,7 @@
         <v>103.8515</v>
       </c>
       <c r="E56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
@@ -1730,7 +1731,7 @@
         <v>103.6613</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
@@ -1747,7 +1748,7 @@
         <v>103.61839999999999</v>
       </c>
       <c r="E58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
@@ -1758,7 +1759,7 @@
         <v>120</v>
       </c>
       <c r="E59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
@@ -1769,7 +1770,7 @@
         <v>121</v>
       </c>
       <c r="E60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
@@ -1780,7 +1781,7 @@
         <v>122</v>
       </c>
       <c r="E61" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -1791,7 +1792,7 @@
         <v>123</v>
       </c>
       <c r="E62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
@@ -1802,7 +1803,7 @@
         <v>124</v>
       </c>
       <c r="E63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -1813,7 +1814,7 @@
         <v>125</v>
       </c>
       <c r="E64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>